<commit_message>
Revised to contain more space for a summary
</commit_message>
<xml_diff>
--- a/RA_hour_task_form.xlsx
+++ b/RA_hour_task_form.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="TVwhglMHEgQn6DcMgNGcUAeHoZJs71I0pV9xxGQJY12IlnuAGysnnGQ5/9JYAUDoRvXd/j3125a8t9Q/mkmI8w==" workbookSaltValue="ZjZt2Pp1rLjESvBiIPMyCQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Report Template" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>#</t>
   </si>
@@ -228,25 +228,16 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Github</t>
-  </si>
-  <si>
-    <t>Commits?</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Research Assistant</t>
   </si>
   <si>
-    <t>[Enter Name At Variables Tab]</t>
-  </si>
-  <si>
     <t>Brief Task Description</t>
   </si>
   <si>
     <t>jsykes@nyit.edu</t>
+  </si>
+  <si>
+    <t>[Enter name at variables tab]</t>
   </si>
 </sst>
 </file>
@@ -483,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -521,6 +512,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -533,11 +548,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -567,48 +594,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -927,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:J7"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -947,83 +932,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="str">
+      <c r="A1" s="20" t="str">
         <f>Variables!$B$5</f>
-        <v>[Enter Name At Variables Tab]</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="17" t="str">
+        <v>[Enter name at variables tab]</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="str">
         <f>Variables!$B$4</f>
         <v>Hours Outline</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="str">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="str">
         <f>Variables!$B$2</f>
         <v>New York Institute of Technology</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="str">
+      <c r="A2" s="20" t="str">
         <f ca="1">"Week # " &amp; Variables!$B$10</f>
-        <v>Week # 22</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="str">
+        <v>Week # 23</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="str">
         <f ca="1">"Ending on " &amp; Variables!$B$18</f>
-        <v>Ending on 06/03</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="17" t="str">
+        <v>Ending on 06/10</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="19" t="str">
         <f ca="1">Variables!$B$11 &amp; " " &amp; Variables!$B$8 &amp; " Research"</f>
         <v>Summer 2018 Research</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="str">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="str">
         <f>Variables!$B$3</f>
         <v>School of Engineering and Computing Sciences</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="36"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1038,234 +1021,261 @@
       <c r="D5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="31"/>
+      <c r="B6" s="14"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="31"/>
+      <c r="B7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="31"/>
+      <c r="B8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="31"/>
+      <c r="B9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>5</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="31"/>
+      <c r="B10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>6</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="31"/>
+      <c r="B11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="31"/>
+      <c r="B12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="31"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>9</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="31"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="31"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>11</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="31"/>
-    </row>
-    <row r="17" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>12</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="31"/>
-    </row>
-    <row r="18" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>13</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="31"/>
-    </row>
-    <row r="19" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>14</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="31"/>
-    </row>
-    <row r="20" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>15</v>
       </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="31"/>
-    </row>
-    <row r="21" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>16</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="31"/>
-    </row>
-    <row r="22" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="31"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aGbkB9/4fFiG1JScNaZZYLhqhu3UD+a9yKIfQlPgR2AsQxqKKTLwvW1PoDjrM1NCwC3fyx26pG7MIuoMayAQAw==" saltValue="XmtFGC59AlE1rMAZzsOj3g==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Xs7i7IHlNqseeyW4bzRHU0rnXvynlRRZ587EcIXj8+vjDV8ppKkY7EUotDOFMWY1iTG3R10pZdvi3ZGA3jh7sQ==" saltValue="ZhSh7+nd+le1ZD/7BsJuFQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
-    <protectedRange sqref="A6:K1048576" name="Report Body"/>
+    <protectedRange sqref="A6:D1048576 H6:K1048576 E6:F6 E7:F7 E8:F8 E9:F9 E10:F10 E11:F11 E13:G1048576 E12:F12" name="Report Body"/>
   </protectedRanges>
-  <mergeCells count="29">
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
+  <mergeCells count="28">
+    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="E8:K8"/>
+    <mergeCell ref="E9:K9"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="E11:K11"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A3:K3"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E6:K6"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E20:K20"/>
+    <mergeCell ref="E21:K21"/>
+    <mergeCell ref="E22:K22"/>
+    <mergeCell ref="E15:K15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="E18:K18"/>
+    <mergeCell ref="E19:K19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.2" bottom="0.2" header="0" footer="0"/>
@@ -1296,128 +1306,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="str">
+      <c r="A1" s="20" t="str">
         <f>Variables!$B$5</f>
-        <v>[Enter Name At Variables Tab]</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="17" t="str">
+        <v>[Enter name at variables tab]</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="str">
         <f>Variables!$B$4</f>
         <v>Hours Outline</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="str">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="str">
         <f>Variables!$B$2</f>
         <v>New York Institute of Technology</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="str">
+      <c r="A2" s="20" t="str">
         <f ca="1">"Week # " &amp; Variables!$B$10</f>
-        <v>Week # 22</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="str">
+        <v>Week # 23</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="str">
         <f ca="1">"Ending on " &amp; Variables!$B$18</f>
-        <v>Ending on 06/03</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="17" t="str">
+        <v>Ending on 06/10</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="19" t="str">
         <f ca="1">Variables!$B$11 &amp; " " &amp; Variables!$B$8 &amp; " Semester"</f>
         <v>Summer 2018 Semester</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="str">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="str">
         <f>Variables!$B$3</f>
         <v>School of Engineering and Computing Sciences</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="13"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1464,35 +1474,35 @@
       <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
     </row>
     <row r="11" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="28"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -1503,35 +1513,35 @@
       <c r="A13" s="2">
         <v>5</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>6</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="21"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
     </row>
     <row r="15" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -1542,35 +1552,35 @@
       <c r="A16" s="2">
         <v>8</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="21"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
     </row>
     <row r="17" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>9</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
     </row>
     <row r="18" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
@@ -1612,9 +1622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,8 +1678,8 @@
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>69</v>
+      <c r="B5" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>49</v>
@@ -1694,14 +1704,14 @@
       </c>
       <c r="B7" s="9">
         <f ca="1">NOW()</f>
-        <v>43251.945998379633</v>
+        <v>43258.821440509259</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="8">
         <f ca="1">IF(ISBLANK($B$6),$B$7,$B$6)</f>
-        <v>43251.945998379633</v>
+        <v>43258.821440509259</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1719,7 +1729,7 @@
       </c>
       <c r="B9" s="6">
         <f ca="1">MONTH($D$7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1728,7 +1738,7 @@
       </c>
       <c r="B10" s="6">
         <f ca="1">_xlfn.ISOWEEKNUM($D$7)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1794,7 +1804,7 @@
       </c>
       <c r="B18" s="7" t="str">
         <f ca="1">TEXT($D$7+(7-$B$17),"mm/dd")</f>
-        <v>06/03</v>
+        <v>06/10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1824,7 +1834,7 @@
         <v>61</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1846,7 +1856,7 @@
         <v>61</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>